<commit_message>
Add 1900 Rtd-Bd '09  to git
</commit_message>
<xml_diff>
--- a/oudelijn-2022.xlsx
+++ b/oudelijn-2022.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Code\quickdrive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD5DD219-9746-41F9-B78F-CD67F8FDECFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDC12D80-122B-4ABA-AF03-84B246587713}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1380" windowWidth="21503" windowHeight="12975" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-7200" yWindow="3697" windowWidth="15247" windowHeight="11648" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Spots" sheetId="2" r:id="rId1"/>
@@ -101,7 +101,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="117">
   <si>
     <t>Treinserie</t>
   </si>
@@ -463,6 +463,66 @@
 - 4834 voor speler
 - 4849
 - 6332</t>
+  </si>
+  <si>
+    <t>Radar 12:50
+'- 4847
+- 2238</t>
+  </si>
+  <si>
+    <t>Radar 12:55
+- 5434</t>
+  </si>
+  <si>
+    <t>Radar 13:00
+- 5453
+- 6351
+- 6332</t>
+  </si>
+  <si>
+    <t>Radar 13:05
+- 2245
+- 4834</t>
+  </si>
+  <si>
+    <t>Radar 13:10
+- 4849</t>
+  </si>
+  <si>
+    <t>Radar 13:15</t>
+  </si>
+  <si>
+    <t>Radar 13:20
+- 2240</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Sommer-Strand-Express v2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+9 juli 2022
+13470 -&gt;Zvt
+Zvt a &lt;13:00
+70450 Zvt-&gt;Hlm
+Zvt 13:05~13:10
+Hlm 13:25</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -550,7 +610,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -568,6 +627,9 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -859,7 +921,7 @@
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="3" max="3" width="4.53125" customWidth="1"/>
-    <col min="4" max="4" width="5.19921875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="5.19921875" style="3" customWidth="1"/>
     <col min="6" max="6" width="30.19921875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -893,7 +955,7 @@
       <c r="C2">
         <v>8</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="3">
         <v>41</v>
       </c>
       <c r="E2" t="s">
@@ -913,7 +975,7 @@
       <c r="C3">
         <v>9</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="3">
         <v>35</v>
       </c>
       <c r="E3" t="s">
@@ -933,7 +995,7 @@
       <c r="C4">
         <v>9</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="3">
         <v>44</v>
       </c>
       <c r="E4" t="s">
@@ -953,7 +1015,7 @@
       <c r="C5">
         <v>10</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="3">
         <v>16</v>
       </c>
       <c r="E5" t="s">
@@ -973,7 +1035,7 @@
       <c r="C6">
         <v>10</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="3">
         <v>20</v>
       </c>
       <c r="E6" t="s">
@@ -993,7 +1055,7 @@
       <c r="C7">
         <v>10</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="3">
         <v>24</v>
       </c>
       <c r="E7" t="s">
@@ -1013,7 +1075,7 @@
       <c r="C8">
         <v>10</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="3">
         <v>25</v>
       </c>
       <c r="E8" t="s">
@@ -1033,7 +1095,7 @@
       <c r="C9">
         <v>10</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="3">
         <v>39</v>
       </c>
       <c r="E9" t="s">
@@ -1053,7 +1115,7 @@
       <c r="C10">
         <v>10</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="3">
         <v>47</v>
       </c>
       <c r="E10" t="s">
@@ -1073,7 +1135,7 @@
       <c r="C11">
         <v>10</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11" s="3">
         <v>58</v>
       </c>
       <c r="E11" t="s">
@@ -1093,7 +1155,7 @@
       <c r="C12">
         <v>11</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D12" s="3">
         <v>14</v>
       </c>
       <c r="E12" t="s">
@@ -1113,7 +1175,7 @@
       <c r="C13">
         <v>11</v>
       </c>
-      <c r="D13" s="4">
+      <c r="D13" s="3">
         <v>14</v>
       </c>
       <c r="E13" t="s">
@@ -1133,7 +1195,7 @@
       <c r="C14">
         <v>11</v>
       </c>
-      <c r="D14" s="4">
+      <c r="D14" s="3">
         <v>30</v>
       </c>
       <c r="E14" t="s">
@@ -1153,7 +1215,7 @@
       <c r="C15">
         <v>11</v>
       </c>
-      <c r="D15" s="4">
+      <c r="D15" s="3">
         <v>30</v>
       </c>
       <c r="E15" t="s">
@@ -1173,7 +1235,7 @@
       <c r="C16">
         <v>11</v>
       </c>
-      <c r="D16" s="4">
+      <c r="D16" s="3">
         <v>50</v>
       </c>
       <c r="E16" t="s">
@@ -1193,7 +1255,7 @@
       <c r="C17">
         <v>11</v>
       </c>
-      <c r="D17" s="4">
+      <c r="D17" s="3">
         <v>55</v>
       </c>
       <c r="E17" t="s">
@@ -1213,7 +1275,7 @@
       <c r="C18">
         <v>12</v>
       </c>
-      <c r="D18" s="4">
+      <c r="D18" s="3">
         <v>19</v>
       </c>
       <c r="E18" t="s">
@@ -1233,7 +1295,7 @@
       <c r="C19">
         <v>13</v>
       </c>
-      <c r="D19" s="4">
+      <c r="D19" s="3">
         <v>56</v>
       </c>
       <c r="E19" t="s">
@@ -1253,7 +1315,7 @@
       <c r="C20">
         <v>14</v>
       </c>
-      <c r="D20" s="4">
+      <c r="D20" s="3">
         <v>17</v>
       </c>
       <c r="E20" t="s">
@@ -1273,7 +1335,7 @@
       <c r="C21">
         <v>14</v>
       </c>
-      <c r="D21" s="4">
+      <c r="D21" s="3">
         <v>55</v>
       </c>
       <c r="E21" t="s">
@@ -1293,7 +1355,7 @@
       <c r="C22">
         <v>15</v>
       </c>
-      <c r="D22" s="4">
+      <c r="D22" s="3">
         <v>5</v>
       </c>
       <c r="E22" t="s">
@@ -1313,7 +1375,7 @@
       <c r="C23">
         <v>15</v>
       </c>
-      <c r="D23" s="4">
+      <c r="D23" s="3">
         <v>22</v>
       </c>
       <c r="E23" t="s">
@@ -1333,7 +1395,7 @@
       <c r="C24">
         <v>15</v>
       </c>
-      <c r="D24" s="4">
+      <c r="D24" s="3">
         <v>22</v>
       </c>
       <c r="E24" t="s">
@@ -1353,7 +1415,7 @@
       <c r="C25">
         <v>15</v>
       </c>
-      <c r="D25" s="4">
+      <c r="D25" s="3">
         <v>23</v>
       </c>
       <c r="E25" t="s">
@@ -1373,7 +1435,7 @@
       <c r="C26">
         <v>15</v>
       </c>
-      <c r="D26" s="4">
+      <c r="D26" s="3">
         <v>33</v>
       </c>
       <c r="E26" t="s">
@@ -1393,7 +1455,7 @@
       <c r="C27">
         <v>15</v>
       </c>
-      <c r="D27" s="4">
+      <c r="D27" s="3">
         <v>36</v>
       </c>
       <c r="E27" t="s">
@@ -1413,7 +1475,7 @@
       <c r="C28">
         <v>16</v>
       </c>
-      <c r="D28" s="4">
+      <c r="D28" s="3">
         <v>40</v>
       </c>
       <c r="E28" t="s">
@@ -1433,7 +1495,7 @@
       <c r="C29">
         <v>19</v>
       </c>
-      <c r="D29" s="4">
+      <c r="D29" s="3">
         <v>44</v>
       </c>
       <c r="E29" t="s">
@@ -1457,7 +1519,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
@@ -1634,7 +1696,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A10" s="3">
+      <c r="A10">
         <v>2400</v>
       </c>
       <c r="C10" t="s">
@@ -1651,7 +1713,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A11" s="3">
+      <c r="A11">
         <v>3200</v>
       </c>
       <c r="C11" t="s">
@@ -1668,7 +1730,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A12" s="3">
+      <c r="A12">
         <v>3300</v>
       </c>
       <c r="C12" t="s">
@@ -1685,7 +1747,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A13" s="3">
+      <c r="A13">
         <v>3400</v>
       </c>
       <c r="C13" t="s">
@@ -1702,7 +1764,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A14" s="3">
+      <c r="A14">
         <v>3700</v>
       </c>
       <c r="B14" t="s">
@@ -1722,7 +1784,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A15" s="3">
+      <c r="A15">
         <v>4600</v>
       </c>
       <c r="C15" t="s">
@@ -1739,7 +1801,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A16" s="3">
+      <c r="A16">
         <v>4800</v>
       </c>
       <c r="C16" t="s">
@@ -1756,7 +1818,7 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A17" s="3">
+      <c r="A17">
         <v>5000</v>
       </c>
       <c r="C17" t="s">
@@ -1773,7 +1835,7 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A18" s="3">
+      <c r="A18">
         <v>5100</v>
       </c>
       <c r="C18" t="s">
@@ -1790,7 +1852,7 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A19" s="3">
+      <c r="A19">
         <v>5400</v>
       </c>
       <c r="C19" t="s">
@@ -1824,7 +1886,7 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A21" s="3">
+      <c r="A21">
         <v>6800</v>
       </c>
       <c r="C21" t="s">
@@ -1841,7 +1903,7 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A22" s="3">
+      <c r="A22">
         <v>6900</v>
       </c>
       <c r="C22" t="s">
@@ -1858,7 +1920,7 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A23" s="3">
+      <c r="A23">
         <v>8800</v>
       </c>
       <c r="C23" t="s">
@@ -1875,7 +1937,7 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A24" s="3">
+      <c r="A24">
         <v>8900</v>
       </c>
       <c r="C24" t="s">
@@ -1892,7 +1954,7 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A25" s="3">
+      <c r="A25">
         <v>11700</v>
       </c>
       <c r="C25" t="s">
@@ -1912,7 +1974,7 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A26" s="3">
+      <c r="A26">
         <v>15400</v>
       </c>
       <c r="B26" t="s">
@@ -1920,7 +1982,7 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A27" s="3">
+      <c r="A27">
         <v>22200</v>
       </c>
       <c r="B27" t="s">
@@ -1928,7 +1990,7 @@
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A28" s="3">
+      <c r="A28">
         <v>25400</v>
       </c>
       <c r="B28" t="s">
@@ -1973,111 +2035,111 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B2" s="5">
         <v>3022</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="6" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="71.25" x14ac:dyDescent="0.45">
-      <c r="A5" s="5"/>
-      <c r="B5" s="8" t="s">
+      <c r="A5" s="4"/>
+      <c r="B5" s="7" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="57" x14ac:dyDescent="0.45">
-      <c r="A6" s="5"/>
-      <c r="B6" s="8" t="s">
+      <c r="A6" s="4"/>
+      <c r="B6" s="7" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="114" x14ac:dyDescent="0.45">
-      <c r="A7" s="5"/>
-      <c r="B7" s="8" t="s">
+      <c r="A7" s="4"/>
+      <c r="B7" s="7" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="99.75" x14ac:dyDescent="0.45">
-      <c r="A8" s="5"/>
-      <c r="B8" s="8" t="s">
+      <c r="A8" s="4"/>
+      <c r="B8" s="7" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A9" s="5"/>
-      <c r="B9" s="6"/>
+      <c r="A9" s="4"/>
+      <c r="B9" s="5"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A10" s="5"/>
-      <c r="B10" s="6"/>
+      <c r="A10" s="4"/>
+      <c r="B10" s="5"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="5" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="5" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="6" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="5" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="5" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A16" s="5"/>
+      <c r="A16" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2087,127 +2149,156 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A227BAE0-D981-4DAD-AC7F-3374DAD9329A}">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
-    <col min="2" max="2" width="15.33203125" customWidth="1"/>
+    <col min="2" max="2" width="26.06640625" customWidth="1"/>
+    <col min="3" max="3" width="26.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:3" ht="99.75" x14ac:dyDescent="0.45">
+      <c r="A1" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A2" s="9" t="s">
+      <c r="C1" s="10" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A2" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" ht="57" x14ac:dyDescent="0.45">
-      <c r="A3" s="9" t="s">
+      <c r="C2" s="5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="57" x14ac:dyDescent="0.45">
+      <c r="A3" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="6" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A4" s="9"/>
-      <c r="B4" s="10" t="s">
+      <c r="C3" s="6" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A4" s="8"/>
+      <c r="B4" s="9" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A5" s="9"/>
-      <c r="B5" s="10" t="s">
+      <c r="C4" s="9" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="57" x14ac:dyDescent="0.45">
+      <c r="A5" s="8"/>
+      <c r="B5" s="9" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" ht="99.75" x14ac:dyDescent="0.45">
-      <c r="A6" s="9"/>
-      <c r="B6" s="10" t="s">
+      <c r="C5" s="9" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="99.75" x14ac:dyDescent="0.45">
+      <c r="A6" s="8"/>
+      <c r="B6" s="9" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A7" s="9"/>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A8" s="9"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A9" s="9"/>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A10" s="9" t="s">
+      <c r="C6" s="9" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A7" s="8"/>
+      <c r="C7" s="9" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A8" s="8"/>
+      <c r="C8" s="9" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A9" s="8"/>
+      <c r="C9" s="9" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A10" s="8" t="s">
         <v>95</v>
       </c>
       <c r="B10" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A11" s="9" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A11" s="8" t="s">
         <v>96</v>
       </c>
       <c r="B11" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A12" s="9" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A12" s="8" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A13" s="9" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A13" s="8" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A14" s="9" t="s">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A14" s="8" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A15" s="9" t="s">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A15" s="8" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A16" s="9" t="s">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A16" s="8" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A17" s="9" t="s">
+      <c r="A17" s="8" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A18" s="9" t="s">
+      <c r="A18" s="8" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A19" s="9" t="s">
+      <c r="A19" s="8" t="s">
         <v>101</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2226,7 +2317,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
         <v>72</v>
       </c>
       <c r="B1" t="s">
@@ -2234,80 +2325,80 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="8" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="8" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A4" s="9"/>
+      <c r="A4" s="8"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A5" s="9"/>
+      <c r="A5" s="8"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A6" s="9"/>
+      <c r="A6" s="8"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A7" s="9"/>
+      <c r="A7" s="8"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A8" s="9"/>
+      <c r="A8" s="8"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A9" s="9"/>
+      <c r="A9" s="8"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="8" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="8" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="8" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="8" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="8" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="8" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A16" s="9" t="s">
+      <c r="A16" s="8" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A17" s="9" t="s">
+      <c r="A17" s="8" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A18" s="9" t="s">
+      <c r="A18" s="8" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A19" s="9" t="s">
+      <c r="A19" s="8" t="s">
         <v>101</v>
       </c>
     </row>

</xml_diff>